<commit_message>
Revise before submission to the legal team
</commit_message>
<xml_diff>
--- a/docs/source/_static/examples/main_check.xlsx
+++ b/docs/source/_static/examples/main_check.xlsx
@@ -40,14 +40,16 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <numFmts count="1">
+  <numFmts count="2">
     <numFmt numFmtId="164" formatCode="General"/>
+    <numFmt numFmtId="165" formatCode="#,##0"/>
   </numFmts>
   <fonts count="4">
     <font>
       <sz val="10"/>
       <name val="Arial"/>
       <family val="2"/>
+      <charset val="1"/>
     </font>
     <font>
       <sz val="10"/>
@@ -107,8 +109,20 @@
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="4">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -129,54 +143,94 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:D6"/>
+  <dimension ref="A1:G15"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="150" zoomScaleNormal="150" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="D3" activeCellId="0" sqref="D3"/>
+      <selection pane="topLeft" activeCell="G14" activeCellId="0" sqref="G14"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.53515625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.55078125" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <cols>
+    <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="2" min="1" style="1" width="11.54"/>
+  </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A1" s="0" t="s">
+      <c r="A1" s="2" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="0" t="s">
+      <c r="B1" s="2"/>
+      <c r="C1" s="3" t="s">
         <v>1</v>
       </c>
+      <c r="D1" s="3"/>
     </row>
     <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A2" s="0" t="n">
-        <f aca="false">SUM(A3:A28)</f>
-        <v>1100200</v>
-      </c>
-      <c r="C2" s="0" t="n">
+      <c r="A2" s="2" t="n">
+        <f aca="false">SUM(A3:A29)</f>
+        <v>1602200</v>
+      </c>
+      <c r="B2" s="2"/>
+      <c r="E2" s="2" t="n">
         <f aca="false">A2</f>
-        <v>1100200</v>
-      </c>
-      <c r="D2" s="0" t="n">
-        <f aca="false">C2/1000</f>
-        <v>1100.2</v>
+        <v>1602200</v>
+      </c>
+      <c r="F2" s="3" t="n">
+        <f aca="false">E2/1000</f>
+        <v>1602.2</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A3" s="0" t="n">
+      <c r="A3" s="2" t="n">
         <v>100</v>
       </c>
+      <c r="B3" s="2"/>
     </row>
     <row r="4" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A4" s="0" t="n">
+      <c r="A4" s="2" t="n">
         <v>100000</v>
       </c>
+      <c r="B4" s="2"/>
     </row>
     <row r="5" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A5" s="0" t="n">
+      <c r="A5" s="2" t="n">
         <v>1000000</v>
       </c>
+      <c r="B5" s="2"/>
     </row>
     <row r="6" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A6" s="0" t="n">
+      <c r="A6" s="2" t="n">
+        <v>500000</v>
+      </c>
+      <c r="B6" s="2"/>
+    </row>
+    <row r="7" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A7" s="2" t="n">
         <v>100</v>
+      </c>
+      <c r="B7" s="2"/>
+    </row>
+    <row r="8" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A8" s="1" t="n">
+        <v>2000</v>
+      </c>
+    </row>
+    <row r="13" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B13" s="1" t="n">
+        <v>2100</v>
+      </c>
+      <c r="G13" s="0" t="n">
+        <f aca="false">B13/1000</f>
+        <v>2.1</v>
+      </c>
+    </row>
+    <row r="15" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B15" s="1" t="n">
+        <f aca="false">100000+100+1000000+500000+2100</f>
+        <v>1602200</v>
+      </c>
+      <c r="C15" s="0" t="n">
+        <f aca="false">B15-B13</f>
+        <v>1600100</v>
       </c>
     </row>
   </sheetData>
@@ -195,79 +249,114 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:F6"/>
+  <dimension ref="A1:F14"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="150" zoomScaleNormal="150" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="F2" activeCellId="0" sqref="F2"/>
+      <selection pane="topLeft" activeCell="F12" activeCellId="0" sqref="F12"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.53515625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.55078125" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A1" s="0" t="s">
+      <c r="A1" s="3" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="0" t="s">
+      <c r="B1" s="3" t="s">
         <v>2</v>
       </c>
-      <c r="C1" s="0" t="s">
+      <c r="C1" s="3" t="s">
         <v>1</v>
       </c>
-      <c r="D1" s="0" t="s">
+      <c r="D1" s="3" t="s">
         <v>3</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A2" s="0" t="n">
-        <f aca="false">SUM(A3:A28)</f>
-        <v>311200</v>
-      </c>
-      <c r="B2" s="0" t="n">
+      <c r="A2" s="3" t="n">
+        <f aca="false">SUM(A3:A30)</f>
+        <v>509400</v>
+      </c>
+      <c r="B2" s="3" t="n">
         <v>200</v>
       </c>
-      <c r="C2" s="0" t="n">
-        <f aca="false">SUM(C3:C20)</f>
-        <v>1010</v>
-      </c>
-      <c r="D2" s="0" t="n">
+      <c r="C2" s="3" t="n">
+        <f aca="false">SUM(C3:C22)</f>
+        <v>1008200</v>
+      </c>
+      <c r="D2" s="3" t="n">
         <v>10</v>
       </c>
-      <c r="E2" s="0" t="n">
+      <c r="E2" s="3" t="n">
         <f aca="false">A2-C2</f>
-        <v>310190</v>
-      </c>
-      <c r="F2" s="0" t="n">
+        <v>-498800</v>
+      </c>
+      <c r="F2" s="3" t="n">
         <f aca="false">E2/10000</f>
-        <v>31.019</v>
+        <v>-49.88</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A3" s="0" t="n">
+      <c r="A3" s="3" t="n">
         <v>200000</v>
       </c>
-      <c r="C3" s="0" t="n">
+      <c r="C3" s="3" t="n">
+        <v>10000</v>
+      </c>
+    </row>
+    <row r="4" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A4" s="3" t="n">
+        <v>10000</v>
+      </c>
+      <c r="C4" s="3" t="n">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="5" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A5" s="3" t="n">
+        <v>100000</v>
+      </c>
+      <c r="C5" s="3"/>
+    </row>
+    <row r="6" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A6" s="3" t="n">
+        <v>198000</v>
+      </c>
+      <c r="C6" s="3"/>
+    </row>
+    <row r="7" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A7" s="3" t="n">
+        <v>200</v>
+      </c>
+      <c r="B7" s="3" t="n">
         <v>1000</v>
       </c>
     </row>
-    <row r="4" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A4" s="0" t="n">
-        <v>10000</v>
-      </c>
-      <c r="C4" s="0" t="n">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="5" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A5" s="0" t="n">
-        <v>100000</v>
-      </c>
-      <c r="B5" s="0" t="n">
-        <v>1000</v>
-      </c>
-    </row>
-    <row r="6" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A6" s="0" t="n">
+    <row r="8" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A8" s="3" t="n">
         <v>1200</v>
+      </c>
+    </row>
+    <row r="11" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="F11" s="0" t="n">
+        <f aca="false">1800/10000</f>
+        <v>0.18</v>
+      </c>
+    </row>
+    <row r="12" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="C12" s="0" t="n">
+        <v>1800</v>
+      </c>
+    </row>
+    <row r="13" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="C13" s="0" t="n">
+        <f aca="false">210000+298000-750+1900-10000-100</f>
+        <v>499050</v>
+      </c>
+    </row>
+    <row r="14" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="C14" s="0" t="n">
+        <f aca="false">C13-C12</f>
+        <v>497250</v>
       </c>
     </row>
   </sheetData>
@@ -286,79 +375,84 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:F6"/>
+  <dimension ref="A1:F13"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="150" zoomScaleNormal="150" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="F2" activeCellId="0" sqref="F2"/>
+      <selection pane="topLeft" activeCell="F16" activeCellId="0" sqref="F16"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.53515625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.55078125" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A1" s="0" t="s">
+      <c r="A1" s="3" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="0" t="s">
+      <c r="B1" s="3" t="s">
         <v>2</v>
       </c>
-      <c r="C1" s="0" t="s">
+      <c r="C1" s="3" t="s">
         <v>1</v>
       </c>
-      <c r="D1" s="0" t="s">
+      <c r="D1" s="3" t="s">
         <v>3</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A2" s="0" t="n">
+      <c r="A2" s="3" t="n">
         <f aca="false">SUM(A3:A28)</f>
-        <v>704500</v>
-      </c>
-      <c r="C2" s="0" t="n">
+        <v>500000</v>
+      </c>
+      <c r="C2" s="3" t="n">
         <f aca="false">SUM(C3:C20)</f>
-        <v>50010</v>
-      </c>
-      <c r="D2" s="0" t="n">
+        <v>491000</v>
+      </c>
+      <c r="D2" s="3" t="n">
         <v>10</v>
       </c>
-      <c r="E2" s="0" t="n">
+      <c r="E2" s="3" t="n">
         <f aca="false">A2-C2</f>
-        <v>654490</v>
-      </c>
-      <c r="F2" s="0" t="n">
+        <v>9000</v>
+      </c>
+      <c r="F2" s="3" t="n">
         <f aca="false">E2/20000</f>
-        <v>32.7245</v>
+        <v>0.45</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A3" s="0" t="n">
+      <c r="A3" s="3" t="n">
         <v>500000</v>
       </c>
-      <c r="B3" s="0" t="n">
+      <c r="B3" s="3" t="n">
         <v>500</v>
       </c>
-      <c r="C3" s="0" t="n">
-        <v>50000</v>
-      </c>
+      <c r="C3" s="3"/>
     </row>
     <row r="4" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A4" s="0" t="n">
-        <v>200000</v>
-      </c>
-      <c r="B4" s="0" t="n">
+      <c r="A4" s="3"/>
+      <c r="B4" s="3" t="n">
         <v>2000</v>
       </c>
-      <c r="C4" s="0" t="n">
-        <v>10</v>
-      </c>
+      <c r="C4" s="3"/>
     </row>
     <row r="5" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A5" s="0" t="n">
-        <v>2000</v>
-      </c>
+      <c r="A5" s="3"/>
     </row>
     <row r="6" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A6" s="0" t="n">
-        <v>2500</v>
+      <c r="A6" s="3"/>
+    </row>
+    <row r="12" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="C12" s="0" t="n">
+        <v>400</v>
+      </c>
+      <c r="F12" s="0" t="n">
+        <f aca="false">400/20000</f>
+        <v>0.02</v>
+      </c>
+    </row>
+    <row r="13" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="C13" s="0" t="n">
+        <f aca="false">500000+200+500-10000-100</f>
+        <v>490600</v>
       </c>
     </row>
   </sheetData>

</xml_diff>